<commit_message>
- Added config for optimizer. - Added log - Added statistics in training_result.xlsx
</commit_message>
<xml_diff>
--- a/training_result.xlsx
+++ b/training_result.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3555" yWindow="0" windowWidth="19305" windowHeight="8340"/>
+    <workbookView xWindow="4740" yWindow="0" windowWidth="19305" windowHeight="8340"/>
   </bookViews>
   <sheets>
     <sheet name="house_price" sheetId="2" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="28">
   <si>
     <t>Model</t>
   </si>
@@ -89,32 +89,82 @@
     <t>remark</t>
   </si>
   <si>
-    <t>min: ~ 0.14</t>
-  </si>
-  <si>
-    <t>min: ~0.15</t>
-  </si>
-  <si>
-    <t>min: ~ 0.07994</t>
-  </si>
-  <si>
     <t>result_1</t>
   </si>
   <si>
-    <t>at step: ~1666</t>
-  </si>
-  <si>
-    <t>- in some cases, cost values largely fluctuate</t>
-  </si>
-  <si>
-    <t>- cost values are mainly around 0.07 (best cost)</t>
+    <t>train_ratio</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">data = </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(1445,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 301)
+label = (1445,)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">data = </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(15,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 301)
+label = (15,)</t>
+    </r>
+  </si>
+  <si>
+    <t>result_2</t>
+  </si>
+  <si>
+    <t>result_3</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> time = 0.19213(s);
+time = 0.21214(s);
+time = 0.21915(s);</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -126,6 +176,14 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -229,7 +287,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
@@ -258,7 +316,13 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
@@ -267,20 +331,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -297,66 +349,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>40143</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>19732</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>511969</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>7162</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="8124487" y="400732"/>
-          <a:ext cx="3507920" cy="1130430"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -624,8 +616,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:J20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -633,8 +625,8 @@
     <col min="1" max="1" width="10.42578125" customWidth="1"/>
     <col min="2" max="2" width="19.85546875" customWidth="1"/>
     <col min="3" max="3" width="19.28515625" customWidth="1"/>
-    <col min="5" max="5" width="11.5703125" customWidth="1"/>
-    <col min="6" max="6" width="10.7109375" customWidth="1"/>
+    <col min="5" max="5" width="17.85546875" customWidth="1"/>
+    <col min="6" max="6" width="19.85546875" customWidth="1"/>
     <col min="7" max="7" width="18.28515625" customWidth="1"/>
     <col min="8" max="8" width="18" customWidth="1"/>
     <col min="9" max="9" width="17.7109375" customWidth="1"/>
@@ -646,10 +638,10 @@
       <c r="B2" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="17" t="s">
+      <c r="C2" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="18"/>
+      <c r="D2" s="15"/>
       <c r="E2" s="9" t="s">
         <v>14</v>
       </c>
@@ -670,8 +662,8 @@
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="19" t="s">
-        <v>24</v>
+      <c r="A3" s="16" t="s">
+        <v>21</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>8</v>
@@ -682,27 +674,21 @@
       <c r="D3" s="5">
         <v>100</v>
       </c>
-      <c r="E3" s="14">
-        <v>1458</v>
-      </c>
-      <c r="F3" s="14">
-        <v>2</v>
-      </c>
-      <c r="G3" s="6" t="s">
+      <c r="E3" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="H3" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="J3" s="12" t="s">
+      <c r="F3" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="19" t="s">
         <v>27</v>
       </c>
+      <c r="J3" s="12"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="19"/>
+      <c r="A4" s="16"/>
       <c r="B4" s="6" t="s">
         <v>9</v>
       </c>
@@ -712,19 +698,15 @@
       <c r="D4" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="15"/>
-      <c r="F4" s="15"/>
-      <c r="G4" s="6" t="s">
-        <v>25</v>
-      </c>
+      <c r="E4" s="17"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="6"/>
       <c r="H4" s="6"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="13" t="s">
-        <v>26</v>
-      </c>
+      <c r="I4" s="17"/>
+      <c r="J4" s="13"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="19"/>
+      <c r="A5" s="16"/>
       <c r="B5" s="6" t="s">
         <v>10</v>
       </c>
@@ -734,15 +716,15 @@
       <c r="D5" s="6">
         <v>1E-3</v>
       </c>
-      <c r="E5" s="15"/>
-      <c r="F5" s="15"/>
+      <c r="E5" s="17"/>
+      <c r="F5" s="17"/>
       <c r="G5" s="6"/>
       <c r="H5" s="6"/>
-      <c r="I5" s="3"/>
+      <c r="I5" s="17"/>
       <c r="J5" s="3"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="19"/>
+      <c r="A6" s="16"/>
       <c r="B6" s="6" t="s">
         <v>11</v>
       </c>
@@ -752,15 +734,15 @@
       <c r="D6" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="15"/>
-      <c r="F6" s="15"/>
+      <c r="E6" s="17"/>
+      <c r="F6" s="17"/>
       <c r="G6" s="6"/>
       <c r="H6" s="6"/>
-      <c r="I6" s="3"/>
+      <c r="I6" s="17"/>
       <c r="J6" s="3"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="19"/>
+      <c r="A7" s="16"/>
       <c r="B7" s="6"/>
       <c r="C7" s="6" t="s">
         <v>6</v>
@@ -768,28 +750,32 @@
       <c r="D7" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E7" s="15"/>
-      <c r="F7" s="15"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="17"/>
       <c r="G7" s="6"/>
       <c r="H7" s="6"/>
-      <c r="I7" s="3"/>
+      <c r="I7" s="17"/>
       <c r="J7" s="3"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="19"/>
+      <c r="A8" s="16"/>
       <c r="B8" s="7"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="16"/>
-      <c r="F8" s="16"/>
+      <c r="C8" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="7">
+        <v>0.99</v>
+      </c>
+      <c r="E8" s="18"/>
+      <c r="F8" s="18"/>
       <c r="G8" s="7"/>
       <c r="H8" s="7"/>
-      <c r="I8" s="4"/>
+      <c r="I8" s="18"/>
       <c r="J8" s="4"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="20">
-        <v>2</v>
+      <c r="A9" s="16" t="s">
+        <v>25</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>8</v>
@@ -800,11 +786,11 @@
       <c r="D9" s="5">
         <v>100</v>
       </c>
-      <c r="E9" s="14">
-        <v>1458</v>
-      </c>
-      <c r="F9" s="14">
-        <v>2</v>
+      <c r="E9" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="F9" s="19" t="s">
+        <v>24</v>
       </c>
       <c r="G9" s="6"/>
       <c r="H9" s="6"/>
@@ -812,7 +798,7 @@
       <c r="J9" s="3"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="19"/>
+      <c r="A10" s="16"/>
       <c r="B10" s="6" t="s">
         <v>9</v>
       </c>
@@ -822,15 +808,15 @@
       <c r="D10" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="E10" s="15"/>
-      <c r="F10" s="15"/>
+      <c r="E10" s="17"/>
+      <c r="F10" s="17"/>
       <c r="G10" s="6"/>
       <c r="H10" s="6"/>
       <c r="I10" s="3"/>
       <c r="J10" s="3"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="19"/>
+      <c r="A11" s="16"/>
       <c r="B11" s="6" t="s">
         <v>10</v>
       </c>
@@ -840,15 +826,15 @@
       <c r="D11" s="6">
         <v>1E-3</v>
       </c>
-      <c r="E11" s="15"/>
-      <c r="F11" s="15"/>
+      <c r="E11" s="17"/>
+      <c r="F11" s="17"/>
       <c r="G11" s="6"/>
       <c r="H11" s="6"/>
       <c r="I11" s="3"/>
       <c r="J11" s="3"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="19"/>
+      <c r="A12" s="16"/>
       <c r="B12" s="6" t="s">
         <v>11</v>
       </c>
@@ -858,15 +844,15 @@
       <c r="D12" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E12" s="15"/>
-      <c r="F12" s="15"/>
+      <c r="E12" s="17"/>
+      <c r="F12" s="17"/>
       <c r="G12" s="6"/>
       <c r="H12" s="6"/>
       <c r="I12" s="3"/>
       <c r="J12" s="3"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="19"/>
+      <c r="A13" s="16"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6" t="s">
         <v>6</v>
@@ -874,28 +860,32 @@
       <c r="D13" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E13" s="15"/>
-      <c r="F13" s="15"/>
+      <c r="E13" s="17"/>
+      <c r="F13" s="17"/>
       <c r="G13" s="6"/>
       <c r="H13" s="6"/>
       <c r="I13" s="3"/>
       <c r="J13" s="3"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="21"/>
+      <c r="A14" s="16"/>
       <c r="B14" s="7"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="16"/>
-      <c r="F14" s="16"/>
+      <c r="C14" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D14" s="7">
+        <v>0.99</v>
+      </c>
+      <c r="E14" s="18"/>
+      <c r="F14" s="18"/>
       <c r="G14" s="7"/>
       <c r="H14" s="7"/>
       <c r="I14" s="4"/>
       <c r="J14" s="4"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="19">
-        <v>3</v>
+      <c r="A15" s="16" t="s">
+        <v>26</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>8</v>
@@ -906,11 +896,11 @@
       <c r="D15" s="5">
         <v>100</v>
       </c>
-      <c r="E15" s="14">
-        <v>1458</v>
-      </c>
-      <c r="F15" s="14">
-        <v>2</v>
+      <c r="E15" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="F15" s="19" t="s">
+        <v>24</v>
       </c>
       <c r="G15" s="6"/>
       <c r="H15" s="6"/>
@@ -918,7 +908,7 @@
       <c r="J15" s="2"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="19"/>
+      <c r="A16" s="16"/>
       <c r="B16" s="6" t="s">
         <v>9</v>
       </c>
@@ -928,15 +918,15 @@
       <c r="D16" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="E16" s="15"/>
-      <c r="F16" s="15"/>
+      <c r="E16" s="17"/>
+      <c r="F16" s="17"/>
       <c r="G16" s="6"/>
       <c r="H16" s="6"/>
       <c r="I16" s="3"/>
       <c r="J16" s="3"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="19"/>
+      <c r="A17" s="16"/>
       <c r="B17" s="6" t="s">
         <v>10</v>
       </c>
@@ -946,15 +936,15 @@
       <c r="D17" s="6">
         <v>1E-3</v>
       </c>
-      <c r="E17" s="15"/>
-      <c r="F17" s="15"/>
+      <c r="E17" s="17"/>
+      <c r="F17" s="17"/>
       <c r="G17" s="6"/>
       <c r="H17" s="6"/>
       <c r="I17" s="3"/>
       <c r="J17" s="3"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="19"/>
+      <c r="A18" s="16"/>
       <c r="B18" s="6" t="s">
         <v>11</v>
       </c>
@@ -964,15 +954,15 @@
       <c r="D18" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E18" s="15"/>
-      <c r="F18" s="15"/>
+      <c r="E18" s="17"/>
+      <c r="F18" s="17"/>
       <c r="G18" s="6"/>
       <c r="H18" s="6"/>
       <c r="I18" s="3"/>
       <c r="J18" s="3"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="19"/>
+      <c r="A19" s="16"/>
       <c r="B19" s="6"/>
       <c r="C19" s="6" t="s">
         <v>6</v>
@@ -980,40 +970,44 @@
       <c r="D19" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E19" s="15"/>
-      <c r="F19" s="15"/>
+      <c r="E19" s="17"/>
+      <c r="F19" s="17"/>
       <c r="G19" s="6"/>
       <c r="H19" s="6"/>
       <c r="I19" s="3"/>
       <c r="J19" s="3"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="21"/>
+      <c r="A20" s="16"/>
       <c r="B20" s="7"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="7"/>
-      <c r="E20" s="16"/>
-      <c r="F20" s="16"/>
+      <c r="C20" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D20" s="7">
+        <v>0.99</v>
+      </c>
+      <c r="E20" s="18"/>
+      <c r="F20" s="18"/>
       <c r="G20" s="7"/>
       <c r="H20" s="7"/>
       <c r="I20" s="4"/>
       <c r="J20" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="11">
+    <mergeCell ref="I3:I8"/>
+    <mergeCell ref="F3:F8"/>
+    <mergeCell ref="E9:E14"/>
+    <mergeCell ref="F9:F14"/>
+    <mergeCell ref="E15:E20"/>
+    <mergeCell ref="F15:F20"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="A3:A8"/>
     <mergeCell ref="A9:A14"/>
     <mergeCell ref="A15:A20"/>
     <mergeCell ref="E3:E8"/>
-    <mergeCell ref="F3:F8"/>
-    <mergeCell ref="E9:E14"/>
-    <mergeCell ref="F9:F14"/>
-    <mergeCell ref="E15:E20"/>
-    <mergeCell ref="F15:F20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
- Added read_test_data function. - Added run file. - Updated training_result.xlsx
</commit_message>
<xml_diff>
--- a/training_result.xlsx
+++ b/training_result.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="4740" yWindow="0" windowWidth="19305" windowHeight="8340"/>
+    <workbookView xWindow="5925" yWindow="0" windowWidth="19305" windowHeight="8340"/>
   </bookViews>
   <sheets>
     <sheet name="house_price" sheetId="2" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="36">
   <si>
     <t>Model</t>
   </si>
@@ -47,9 +47,6 @@
     <t>l2_beta</t>
   </si>
   <si>
-    <t>tCost</t>
-  </si>
-  <si>
     <t>fc1_512</t>
   </si>
   <si>
@@ -72,9 +69,6 @@
   </si>
   <si>
     <t>num_eval</t>
-  </si>
-  <si>
-    <t>eCost</t>
   </si>
   <si>
     <t>time</t>
@@ -158,6 +152,36 @@
     <t xml:space="preserve"> time = 0.19213(s);
 time = 0.21214(s);
 time = 0.21915(s);</t>
+  </si>
+  <si>
+    <t>tCost/step</t>
+  </si>
+  <si>
+    <t>eCost/step</t>
+  </si>
+  <si>
+    <t>min: 0.37479/7628</t>
+  </si>
+  <si>
+    <t>start: 9.64/1</t>
+  </si>
+  <si>
+    <t>min: 0.3641/9831</t>
+  </si>
+  <si>
+    <t>0.14711(s)</t>
+  </si>
+  <si>
+    <t>0.15962(s)</t>
+  </si>
+  <si>
+    <t>0.14811(s)</t>
+  </si>
+  <si>
+    <t>0.14561(s)</t>
+  </si>
+  <si>
+    <t>0.15695(s)</t>
   </si>
 </sst>
 </file>
@@ -287,7 +311,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
@@ -316,6 +340,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -325,14 +358,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -617,7 +644,7 @@
   <dimension ref="A2:J20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -638,35 +665,35 @@
       <c r="B2" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="C2" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="15"/>
+      <c r="D2" s="18"/>
       <c r="E2" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="G2" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="I2" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="J2" s="10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>7</v>
-      </c>
-      <c r="H2" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="I2" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="J2" s="10" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>8</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>2</v>
@@ -674,41 +701,45 @@
       <c r="D3" s="5">
         <v>100</v>
       </c>
-      <c r="E3" s="19" t="s">
-        <v>23</v>
-      </c>
-      <c r="F3" s="19" t="s">
-        <v>24</v>
+      <c r="E3" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="F3" s="14" t="s">
+        <v>22</v>
       </c>
       <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="19" t="s">
-        <v>27</v>
+      <c r="H3" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="I3" s="14" t="s">
+        <v>25</v>
       </c>
       <c r="J3" s="12"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="16"/>
+      <c r="A4" s="19"/>
       <c r="B4" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>3</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" s="17"/>
-      <c r="F4" s="17"/>
+        <v>12</v>
+      </c>
+      <c r="E4" s="15"/>
+      <c r="F4" s="15"/>
       <c r="G4" s="6"/>
-      <c r="H4" s="6"/>
-      <c r="I4" s="17"/>
+      <c r="H4" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="I4" s="15"/>
       <c r="J4" s="13"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="16"/>
+      <c r="A5" s="19"/>
       <c r="B5" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>4</v>
@@ -716,69 +747,69 @@
       <c r="D5" s="6">
         <v>1E-3</v>
       </c>
-      <c r="E5" s="17"/>
-      <c r="F5" s="17"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="15"/>
       <c r="G5" s="6"/>
       <c r="H5" s="6"/>
-      <c r="I5" s="17"/>
+      <c r="I5" s="15"/>
       <c r="J5" s="3"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="16"/>
+      <c r="A6" s="19"/>
       <c r="B6" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>5</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E6" s="17"/>
-      <c r="F6" s="17"/>
+        <v>11</v>
+      </c>
+      <c r="E6" s="15"/>
+      <c r="F6" s="15"/>
       <c r="G6" s="6"/>
       <c r="H6" s="6"/>
-      <c r="I6" s="17"/>
+      <c r="I6" s="15"/>
       <c r="J6" s="3"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="16"/>
+      <c r="A7" s="19"/>
       <c r="B7" s="6"/>
       <c r="C7" s="6" t="s">
         <v>6</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E7" s="17"/>
-      <c r="F7" s="17"/>
+        <v>11</v>
+      </c>
+      <c r="E7" s="15"/>
+      <c r="F7" s="15"/>
       <c r="G7" s="6"/>
       <c r="H7" s="6"/>
-      <c r="I7" s="17"/>
+      <c r="I7" s="15"/>
       <c r="J7" s="3"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="16"/>
+      <c r="A8" s="19"/>
       <c r="B8" s="7"/>
       <c r="C8" s="7" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D8" s="7">
         <v>0.99</v>
       </c>
-      <c r="E8" s="18"/>
-      <c r="F8" s="18"/>
+      <c r="E8" s="16"/>
+      <c r="F8" s="16"/>
       <c r="G8" s="7"/>
       <c r="H8" s="7"/>
-      <c r="I8" s="18"/>
+      <c r="I8" s="16"/>
       <c r="J8" s="4"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="16" t="s">
-        <v>25</v>
+      <c r="A9" s="19" t="s">
+        <v>23</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>2</v>
@@ -786,39 +817,45 @@
       <c r="D9" s="5">
         <v>100</v>
       </c>
-      <c r="E9" s="19" t="s">
-        <v>23</v>
-      </c>
-      <c r="F9" s="19" t="s">
-        <v>24</v>
+      <c r="E9" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="F9" s="14" t="s">
+        <v>22</v>
       </c>
       <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
-      <c r="I9" s="2"/>
+      <c r="H9" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="I9" t="s">
+        <v>31</v>
+      </c>
       <c r="J9" s="3"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="16"/>
+      <c r="A10" s="19"/>
       <c r="B10" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C10" s="6" t="s">
         <v>3</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="E10" s="17"/>
-      <c r="F10" s="17"/>
+        <v>16</v>
+      </c>
+      <c r="E10" s="15"/>
+      <c r="F10" s="15"/>
       <c r="G10" s="6"/>
       <c r="H10" s="6"/>
-      <c r="I10" s="3"/>
+      <c r="I10" t="s">
+        <v>32</v>
+      </c>
       <c r="J10" s="3"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="16"/>
+      <c r="A11" s="19"/>
       <c r="B11" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C11" s="6" t="s">
         <v>4</v>
@@ -826,69 +863,75 @@
       <c r="D11" s="6">
         <v>1E-3</v>
       </c>
-      <c r="E11" s="17"/>
-      <c r="F11" s="17"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="15"/>
       <c r="G11" s="6"/>
       <c r="H11" s="6"/>
-      <c r="I11" s="3"/>
+      <c r="I11" t="s">
+        <v>33</v>
+      </c>
       <c r="J11" s="3"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="16"/>
+      <c r="A12" s="19"/>
       <c r="B12" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C12" s="6" t="s">
         <v>5</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E12" s="17"/>
-      <c r="F12" s="17"/>
+        <v>11</v>
+      </c>
+      <c r="E12" s="15"/>
+      <c r="F12" s="15"/>
       <c r="G12" s="6"/>
       <c r="H12" s="6"/>
-      <c r="I12" s="3"/>
+      <c r="I12" t="s">
+        <v>34</v>
+      </c>
       <c r="J12" s="3"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="16"/>
+      <c r="A13" s="19"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6" t="s">
         <v>6</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E13" s="17"/>
-      <c r="F13" s="17"/>
+        <v>11</v>
+      </c>
+      <c r="E13" s="15"/>
+      <c r="F13" s="15"/>
       <c r="G13" s="6"/>
       <c r="H13" s="6"/>
-      <c r="I13" s="3"/>
+      <c r="I13" t="s">
+        <v>35</v>
+      </c>
       <c r="J13" s="3"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="16"/>
+      <c r="A14" s="19"/>
       <c r="B14" s="7"/>
       <c r="C14" s="7" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D14" s="7">
         <v>0.99</v>
       </c>
-      <c r="E14" s="18"/>
-      <c r="F14" s="18"/>
+      <c r="E14" s="16"/>
+      <c r="F14" s="16"/>
       <c r="G14" s="7"/>
       <c r="H14" s="7"/>
       <c r="I14" s="4"/>
       <c r="J14" s="4"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="16" t="s">
-        <v>26</v>
+      <c r="A15" s="19" t="s">
+        <v>24</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>2</v>
@@ -896,11 +939,11 @@
       <c r="D15" s="5">
         <v>100</v>
       </c>
-      <c r="E15" s="19" t="s">
-        <v>23</v>
-      </c>
-      <c r="F15" s="19" t="s">
-        <v>24</v>
+      <c r="E15" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="F15" s="14" t="s">
+        <v>22</v>
       </c>
       <c r="G15" s="6"/>
       <c r="H15" s="6"/>
@@ -908,27 +951,27 @@
       <c r="J15" s="2"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="16"/>
+      <c r="A16" s="19"/>
       <c r="B16" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C16" s="6" t="s">
         <v>3</v>
       </c>
       <c r="D16" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="E16" s="17"/>
-      <c r="F16" s="17"/>
+        <v>17</v>
+      </c>
+      <c r="E16" s="15"/>
+      <c r="F16" s="15"/>
       <c r="G16" s="6"/>
       <c r="H16" s="6"/>
       <c r="I16" s="3"/>
       <c r="J16" s="3"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="16"/>
+      <c r="A17" s="19"/>
       <c r="B17" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C17" s="6" t="s">
         <v>4</v>
@@ -936,58 +979,58 @@
       <c r="D17" s="6">
         <v>1E-3</v>
       </c>
-      <c r="E17" s="17"/>
-      <c r="F17" s="17"/>
+      <c r="E17" s="15"/>
+      <c r="F17" s="15"/>
       <c r="G17" s="6"/>
       <c r="H17" s="6"/>
       <c r="I17" s="3"/>
       <c r="J17" s="3"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="16"/>
+      <c r="A18" s="19"/>
       <c r="B18" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C18" s="6" t="s">
         <v>5</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E18" s="17"/>
-      <c r="F18" s="17"/>
+        <v>11</v>
+      </c>
+      <c r="E18" s="15"/>
+      <c r="F18" s="15"/>
       <c r="G18" s="6"/>
       <c r="H18" s="6"/>
       <c r="I18" s="3"/>
       <c r="J18" s="3"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="16"/>
+      <c r="A19" s="19"/>
       <c r="B19" s="6"/>
       <c r="C19" s="6" t="s">
         <v>6</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E19" s="17"/>
-      <c r="F19" s="17"/>
+        <v>11</v>
+      </c>
+      <c r="E19" s="15"/>
+      <c r="F19" s="15"/>
       <c r="G19" s="6"/>
       <c r="H19" s="6"/>
       <c r="I19" s="3"/>
       <c r="J19" s="3"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="16"/>
+      <c r="A20" s="19"/>
       <c r="B20" s="7"/>
       <c r="C20" s="7" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D20" s="7">
         <v>0.99</v>
       </c>
-      <c r="E20" s="18"/>
-      <c r="F20" s="18"/>
+      <c r="E20" s="16"/>
+      <c r="F20" s="16"/>
       <c r="G20" s="7"/>
       <c r="H20" s="7"/>
       <c r="I20" s="4"/>
@@ -995,17 +1038,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="A3:A8"/>
+    <mergeCell ref="A9:A14"/>
+    <mergeCell ref="A15:A20"/>
+    <mergeCell ref="E3:E8"/>
     <mergeCell ref="I3:I8"/>
     <mergeCell ref="F3:F8"/>
     <mergeCell ref="E9:E14"/>
     <mergeCell ref="F9:F14"/>
     <mergeCell ref="E15:E20"/>
     <mergeCell ref="F15:F20"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="A3:A8"/>
-    <mergeCell ref="A9:A14"/>
-    <mergeCell ref="A15:A20"/>
-    <mergeCell ref="E3:E8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
- Updated hyperparams. - Edited data reading
</commit_message>
<xml_diff>
--- a/training_result.xlsx
+++ b/training_result.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="5925" yWindow="0" windowWidth="19305" windowHeight="8340"/>
+    <workbookView xWindow="15405" yWindow="0" windowWidth="19305" windowHeight="8340"/>
   </bookViews>
   <sheets>
     <sheet name="house_price" sheetId="2" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="81">
   <si>
     <t>Model</t>
   </si>
@@ -183,12 +183,243 @@
   <si>
     <t>0.15695(s)</t>
   </si>
+  <si>
+    <t>mins: ~0.5</t>
+  </si>
+  <si>
+    <t>prediction on kaggle is approximately same to eCost</t>
+  </si>
+  <si>
+    <t>==&gt; try to optimize eCost as small as possible</t>
+  </si>
+  <si>
+    <t>result_4</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">data = </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(1168,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 301)
+label = (1168,)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">data = </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(292,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 301)
+label = (292,)</t>
+    </r>
+  </si>
+  <si>
+    <t>min: 0.306/8779</t>
+  </si>
+  <si>
+    <t>min eCost was around 0.03</t>
+  </si>
+  <si>
+    <t>min: 0.0794/9618</t>
+  </si>
+  <si>
+    <t>If we would like to get eCost small as tCost --&gt; add more data will be helpful</t>
+  </si>
+  <si>
+    <t>0.24816(s)</t>
+  </si>
+  <si>
+    <t>0.18562(s)</t>
+  </si>
+  <si>
+    <t>0.21214(s)</t>
+  </si>
+  <si>
+    <t>0.22765(s)</t>
+  </si>
+  <si>
+    <t>result_5</t>
+  </si>
+  <si>
+    <t>min: ~0.31/9825</t>
+  </si>
+  <si>
+    <t>min: 0.29/9879</t>
+  </si>
+  <si>
+    <t>min eCost was around 0.31</t>
+  </si>
+  <si>
+    <t>result_6</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ==&gt; add more data to get smaller eCost</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">data = </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(1387,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 301)
+label = (1387,)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">data = </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(73,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 301)
+label = (73,)</t>
+    </r>
+  </si>
+  <si>
+    <t>min: 0.3145/9680</t>
+  </si>
+  <si>
+    <t>min: 0.079/9070</t>
+  </si>
+  <si>
+    <t>in this case, adding more training data was not helpful ==&gt; why ????</t>
+  </si>
+  <si>
+    <t>even we added more training data than previous tests, min eCost was similar to previous ones</t>
+  </si>
+  <si>
+    <t>=&gt; The reason may be model !!!!</t>
+  </si>
+  <si>
+    <t>result_7</t>
+  </si>
+  <si>
+    <t>fc1_128</t>
+  </si>
+  <si>
+    <t>fc2_64</t>
+  </si>
+  <si>
+    <t>fc3_1</t>
+  </si>
+  <si>
+    <t>min: ~0.08</t>
+  </si>
+  <si>
+    <t>min: ~0.326</t>
+  </si>
+  <si>
+    <t>result_8</t>
+  </si>
+  <si>
+    <t>fc 2048</t>
+  </si>
+  <si>
+    <t>fc 1024</t>
+  </si>
+  <si>
+    <t>fc 512</t>
+  </si>
+  <si>
+    <t>fc 256</t>
+  </si>
+  <si>
+    <t>fc 128</t>
+  </si>
+  <si>
+    <t>fc 64 -&gt; fc 1</t>
+  </si>
+  <si>
+    <t>min: ~0.31</t>
+  </si>
+  <si>
+    <t>min: 0.079</t>
+  </si>
+  <si>
+    <t>Even a complex model was applied, but eCost was not improved much, same as before</t>
+  </si>
+  <si>
+    <t>==&gt; more training data (above), more complex model were not helpful</t>
+  </si>
+  <si>
+    <t>==&gt; The reason may be data processing</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -208,6 +439,19 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -311,7 +555,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
@@ -335,11 +579,42 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -355,12 +630,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -641,10 +911,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:J20"/>
+  <dimension ref="A1:J52"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" topLeftCell="C32" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J40" sqref="J40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -657,398 +927,1011 @@
     <col min="7" max="7" width="18.28515625" customWidth="1"/>
     <col min="8" max="8" width="18" customWidth="1"/>
     <col min="9" max="9" width="17.7109375" customWidth="1"/>
-    <col min="10" max="10" width="44.7109375" customWidth="1"/>
+    <col min="10" max="10" width="84.140625" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H1" s="14" t="s">
+        <v>37</v>
+      </c>
+    </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
-      <c r="B2" s="8" t="s">
+      <c r="H2" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="I2" s="14"/>
+      <c r="J2" s="14"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="1"/>
+      <c r="B4" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="17" t="s">
+      <c r="C4" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="18"/>
-      <c r="E2" s="9" t="s">
+      <c r="D4" s="31"/>
+      <c r="E4" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="F4" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="G4" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="H2" s="8" t="s">
+      <c r="H4" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="I2" s="10" t="s">
+      <c r="I4" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="J2" s="10" t="s">
+      <c r="J4" s="10" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="19" t="s">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B5" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C5" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="5">
+      <c r="D5" s="5">
         <v>100</v>
       </c>
-      <c r="E3" s="14" t="s">
+      <c r="E5" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="14" t="s">
+      <c r="F5" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="G3" s="6"/>
-      <c r="H3" s="20" t="s">
+      <c r="G5" s="6"/>
+      <c r="H5" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="I3" s="14" t="s">
+      <c r="I5" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="J3" s="12"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="19"/>
-      <c r="B4" s="6" t="s">
+      <c r="J5" s="11"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="25"/>
+      <c r="B6" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C6" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="11" t="s">
+      <c r="D6" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="15"/>
-      <c r="F4" s="15"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="6" t="s">
+      <c r="E6" s="28"/>
+      <c r="F6" s="28"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="I4" s="15"/>
-      <c r="J4" s="13"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="19"/>
-      <c r="B5" s="6" t="s">
+      <c r="I6" s="28"/>
+      <c r="J6" s="12"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="25"/>
+      <c r="B7" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C7" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D7" s="6">
         <v>1E-3</v>
       </c>
-      <c r="E5" s="15"/>
-      <c r="F5" s="15"/>
-      <c r="G5" s="6"/>
-      <c r="H5" s="6"/>
-      <c r="I5" s="15"/>
-      <c r="J5" s="3"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="19"/>
-      <c r="B6" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6" s="15"/>
-      <c r="F6" s="15"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="6"/>
-      <c r="I6" s="15"/>
-      <c r="J6" s="3"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="19"/>
-      <c r="B7" s="6"/>
-      <c r="C7" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7" s="15"/>
-      <c r="F7" s="15"/>
+      <c r="E7" s="28"/>
+      <c r="F7" s="28"/>
       <c r="G7" s="6"/>
       <c r="H7" s="6"/>
-      <c r="I7" s="15"/>
+      <c r="I7" s="28"/>
       <c r="J7" s="3"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="19"/>
-      <c r="B8" s="7"/>
-      <c r="C8" s="7" t="s">
+      <c r="A8" s="25"/>
+      <c r="B8" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" s="28"/>
+      <c r="F8" s="28"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="28"/>
+      <c r="J8" s="3"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="25"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" s="28"/>
+      <c r="F9" s="28"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="28"/>
+      <c r="J9" s="3"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="25"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="D8" s="7">
+      <c r="D10" s="7">
         <v>0.99</v>
       </c>
-      <c r="E8" s="16"/>
-      <c r="F8" s="16"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="7"/>
-      <c r="I8" s="16"/>
-      <c r="J8" s="4"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="19" t="s">
+      <c r="E10" s="29"/>
+      <c r="F10" s="29"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
+      <c r="I10" s="29"/>
+      <c r="J10" s="4"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B11" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C11" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D9" s="5">
+      <c r="D11" s="5">
         <v>100</v>
       </c>
-      <c r="E9" s="14" t="s">
+      <c r="E11" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="F9" s="14" t="s">
+      <c r="F11" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="G9" s="6"/>
-      <c r="H9" s="20" t="s">
+      <c r="G11" s="6"/>
+      <c r="H11" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="I9" t="s">
+      <c r="I11" t="s">
         <v>31</v>
       </c>
-      <c r="J9" s="3"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="19"/>
-      <c r="B10" s="6" t="s">
+      <c r="J11" s="3"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="25"/>
+      <c r="B12" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C12" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D10" s="11" t="s">
+      <c r="D12" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="E10" s="15"/>
-      <c r="F10" s="15"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
-      <c r="I10" t="s">
-        <v>32</v>
-      </c>
-      <c r="J10" s="3"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="19"/>
-      <c r="B11" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D11" s="6">
-        <v>1E-3</v>
-      </c>
-      <c r="E11" s="15"/>
-      <c r="F11" s="15"/>
-      <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
-      <c r="I11" t="s">
-        <v>33</v>
-      </c>
-      <c r="J11" s="3"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="19"/>
-      <c r="B12" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="D12" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E12" s="15"/>
-      <c r="F12" s="15"/>
+      <c r="E12" s="28"/>
+      <c r="F12" s="28"/>
       <c r="G12" s="6"/>
       <c r="H12" s="6"/>
       <c r="I12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J12" s="3"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="19"/>
-      <c r="B13" s="6"/>
+      <c r="A13" s="25"/>
+      <c r="B13" s="6" t="s">
+        <v>9</v>
+      </c>
       <c r="C13" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E13" s="15"/>
-      <c r="F13" s="15"/>
+        <v>4</v>
+      </c>
+      <c r="D13" s="6">
+        <v>1E-3</v>
+      </c>
+      <c r="E13" s="28"/>
+      <c r="F13" s="28"/>
       <c r="G13" s="6"/>
       <c r="H13" s="6"/>
       <c r="I13" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="J13" s="3"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="19"/>
-      <c r="B14" s="7"/>
-      <c r="C14" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D14" s="7">
-        <v>0.99</v>
-      </c>
-      <c r="E14" s="16"/>
-      <c r="F14" s="16"/>
-      <c r="G14" s="7"/>
-      <c r="H14" s="7"/>
-      <c r="I14" s="4"/>
-      <c r="J14" s="4"/>
+      <c r="A14" s="25"/>
+      <c r="B14" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E14" s="28"/>
+      <c r="F14" s="28"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
+      <c r="I14" t="s">
+        <v>34</v>
+      </c>
+      <c r="J14" s="3"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="19" t="s">
-        <v>24</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="D15" s="5">
-        <v>100</v>
-      </c>
-      <c r="E15" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="F15" s="14" t="s">
-        <v>22</v>
-      </c>
+      <c r="A15" s="25"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E15" s="28"/>
+      <c r="F15" s="28"/>
       <c r="G15" s="6"/>
       <c r="H15" s="6"/>
-      <c r="I15" s="2"/>
-      <c r="J15" s="2"/>
+      <c r="I15" t="s">
+        <v>35</v>
+      </c>
+      <c r="J15" s="3"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="19"/>
-      <c r="B16" s="6" t="s">
+      <c r="A16" s="26"/>
+      <c r="B16" s="7"/>
+      <c r="C16" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D16" s="7">
+        <v>0.99</v>
+      </c>
+      <c r="E16" s="29"/>
+      <c r="F16" s="29"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="7"/>
+      <c r="I16" s="4"/>
+      <c r="J16" s="4"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D17" s="5">
+        <v>500</v>
+      </c>
+      <c r="E17" s="27" t="s">
+        <v>21</v>
+      </c>
+      <c r="F17" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="G17" s="6"/>
+      <c r="H17" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="I17" s="2"/>
+      <c r="J17" s="2"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="25"/>
+      <c r="B18" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C16" s="6" t="s">
+      <c r="C18" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D16" s="11" t="s">
+      <c r="D18" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="E16" s="15"/>
-      <c r="F16" s="15"/>
-      <c r="G16" s="6"/>
-      <c r="H16" s="6"/>
-      <c r="I16" s="3"/>
-      <c r="J16" s="3"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="19"/>
-      <c r="B17" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C17" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D17" s="6">
-        <v>1E-3</v>
-      </c>
-      <c r="E17" s="15"/>
-      <c r="F17" s="15"/>
-      <c r="G17" s="6"/>
-      <c r="H17" s="6"/>
-      <c r="I17" s="3"/>
-      <c r="J17" s="3"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="19"/>
-      <c r="B18" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C18" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="D18" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E18" s="15"/>
-      <c r="F18" s="15"/>
+      <c r="E18" s="28"/>
+      <c r="F18" s="28"/>
       <c r="G18" s="6"/>
       <c r="H18" s="6"/>
       <c r="I18" s="3"/>
       <c r="J18" s="3"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="19"/>
-      <c r="B19" s="6"/>
+      <c r="A19" s="25"/>
+      <c r="B19" s="6" t="s">
+        <v>9</v>
+      </c>
       <c r="C19" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D19" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E19" s="15"/>
-      <c r="F19" s="15"/>
+        <v>4</v>
+      </c>
+      <c r="D19" s="6">
+        <v>1E-3</v>
+      </c>
+      <c r="E19" s="28"/>
+      <c r="F19" s="28"/>
       <c r="G19" s="6"/>
       <c r="H19" s="6"/>
       <c r="I19" s="3"/>
       <c r="J19" s="3"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="19"/>
-      <c r="B20" s="7"/>
-      <c r="C20" s="7" t="s">
+      <c r="A20" s="25"/>
+      <c r="B20" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E20" s="28"/>
+      <c r="F20" s="28"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="6"/>
+      <c r="I20" s="3"/>
+      <c r="J20" s="3"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" s="25"/>
+      <c r="B21" s="6"/>
+      <c r="C21" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E21" s="28"/>
+      <c r="F21" s="28"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="6"/>
+      <c r="I21" s="3"/>
+      <c r="J21" s="3"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" s="25"/>
+      <c r="B22" s="7"/>
+      <c r="C22" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="D20" s="7">
+      <c r="D22" s="7">
         <v>0.99</v>
       </c>
-      <c r="E20" s="16"/>
-      <c r="F20" s="16"/>
-      <c r="G20" s="7"/>
-      <c r="H20" s="7"/>
-      <c r="I20" s="4"/>
-      <c r="J20" s="4"/>
+      <c r="E22" s="29"/>
+      <c r="F22" s="29"/>
+      <c r="G22" s="7"/>
+      <c r="H22" s="7"/>
+      <c r="I22" s="4"/>
+      <c r="J22" s="4"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D23" s="18">
+        <v>500</v>
+      </c>
+      <c r="E23" s="27" t="s">
+        <v>40</v>
+      </c>
+      <c r="F23" s="27" t="s">
+        <v>41</v>
+      </c>
+      <c r="G23" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="H23" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="I23" t="s">
+        <v>46</v>
+      </c>
+      <c r="J23" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" s="25"/>
+      <c r="B24" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D24" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="E24" s="28"/>
+      <c r="F24" s="28"/>
+      <c r="G24" s="6"/>
+      <c r="H24" s="6"/>
+      <c r="I24" t="s">
+        <v>47</v>
+      </c>
+      <c r="J24" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" s="25"/>
+      <c r="B25" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D25" s="6">
+        <v>1E-3</v>
+      </c>
+      <c r="E25" s="28"/>
+      <c r="F25" s="28"/>
+      <c r="G25" s="6"/>
+      <c r="H25" s="6"/>
+      <c r="I25" t="s">
+        <v>48</v>
+      </c>
+      <c r="J25" s="3"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" s="25"/>
+      <c r="B26" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E26" s="28"/>
+      <c r="F26" s="28"/>
+      <c r="G26" s="6"/>
+      <c r="H26" s="6"/>
+      <c r="I26" t="s">
+        <v>49</v>
+      </c>
+      <c r="J26" s="3"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" s="25"/>
+      <c r="B27" s="6"/>
+      <c r="C27" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E27" s="28"/>
+      <c r="F27" s="28"/>
+      <c r="G27" s="6"/>
+      <c r="H27" s="6"/>
+      <c r="I27" s="3"/>
+      <c r="J27" s="3"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" s="26"/>
+      <c r="B28" s="7"/>
+      <c r="C28" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D28" s="19">
+        <v>0.8</v>
+      </c>
+      <c r="E28" s="29"/>
+      <c r="F28" s="29"/>
+      <c r="G28" s="7"/>
+      <c r="H28" s="7"/>
+      <c r="I28" s="4"/>
+      <c r="J28" s="4"/>
+    </row>
+    <row r="29" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="24" t="s">
+        <v>50</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D29" s="20">
+        <v>500</v>
+      </c>
+      <c r="E29" s="27" t="s">
+        <v>40</v>
+      </c>
+      <c r="F29" s="27" t="s">
+        <v>41</v>
+      </c>
+      <c r="G29" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="H29" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="J29" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" s="25"/>
+      <c r="B30" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D30" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="E30" s="28"/>
+      <c r="F30" s="28"/>
+      <c r="G30" s="6"/>
+      <c r="H30" s="6"/>
+      <c r="J30" s="12" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31" s="25"/>
+      <c r="B31" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D31" s="17">
+        <v>1E-4</v>
+      </c>
+      <c r="E31" s="28"/>
+      <c r="F31" s="28"/>
+      <c r="G31" s="6"/>
+      <c r="H31" s="6"/>
+      <c r="J31" s="3"/>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A32" s="25"/>
+      <c r="B32" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D32" s="17">
+        <v>0.9</v>
+      </c>
+      <c r="E32" s="28"/>
+      <c r="F32" s="28"/>
+      <c r="G32" s="6"/>
+      <c r="H32" s="6"/>
+      <c r="J32" s="3"/>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A33" s="25"/>
+      <c r="B33" s="6"/>
+      <c r="C33" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D33" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E33" s="28"/>
+      <c r="F33" s="28"/>
+      <c r="G33" s="6"/>
+      <c r="H33" s="6"/>
+      <c r="I33" s="3"/>
+      <c r="J33" s="3"/>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A34" s="26"/>
+      <c r="B34" s="7"/>
+      <c r="C34" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D34" s="21">
+        <v>0.8</v>
+      </c>
+      <c r="E34" s="29"/>
+      <c r="F34" s="29"/>
+      <c r="G34" s="7"/>
+      <c r="H34" s="7"/>
+      <c r="I34" s="4"/>
+      <c r="J34" s="4"/>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A35" s="24" t="s">
+        <v>54</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D35" s="20">
+        <v>500</v>
+      </c>
+      <c r="E35" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="F35" s="27" t="s">
+        <v>57</v>
+      </c>
+      <c r="G35" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="H35" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="J35" s="23" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A36" s="25"/>
+      <c r="B36" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C36" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D36" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="E36" s="28"/>
+      <c r="F36" s="28"/>
+      <c r="G36" s="6"/>
+      <c r="H36" s="6"/>
+      <c r="J36" s="22" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A37" s="25"/>
+      <c r="B37" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C37" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D37" s="16">
+        <v>1E-3</v>
+      </c>
+      <c r="E37" s="28"/>
+      <c r="F37" s="28"/>
+      <c r="G37" s="6"/>
+      <c r="H37" s="6"/>
+      <c r="J37" s="12" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A38" s="25"/>
+      <c r="B38" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C38" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D38" s="16">
+        <v>0</v>
+      </c>
+      <c r="E38" s="28"/>
+      <c r="F38" s="28"/>
+      <c r="G38" s="6"/>
+      <c r="H38" s="6"/>
+      <c r="J38" s="3"/>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A39" s="25"/>
+      <c r="B39" s="6"/>
+      <c r="C39" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D39" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E39" s="28"/>
+      <c r="F39" s="28"/>
+      <c r="G39" s="6"/>
+      <c r="H39" s="6"/>
+      <c r="I39" s="3"/>
+      <c r="J39" s="3"/>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A40" s="26"/>
+      <c r="B40" s="7"/>
+      <c r="C40" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D40" s="19">
+        <v>0.95</v>
+      </c>
+      <c r="E40" s="29"/>
+      <c r="F40" s="29"/>
+      <c r="G40" s="7"/>
+      <c r="H40" s="7"/>
+      <c r="I40" s="4"/>
+      <c r="J40" s="4"/>
+    </row>
+    <row r="41" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="24" t="s">
+        <v>63</v>
+      </c>
+      <c r="B41" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="C41" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D41" s="20">
+        <v>500</v>
+      </c>
+      <c r="E41" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="F41" s="27" t="s">
+        <v>57</v>
+      </c>
+      <c r="G41" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="H41" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="J41" s="23"/>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A42" s="25"/>
+      <c r="B42" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="C42" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D42" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="E42" s="28"/>
+      <c r="F42" s="28"/>
+      <c r="G42" s="6"/>
+      <c r="H42" s="6"/>
+      <c r="J42" s="22"/>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A43" s="25"/>
+      <c r="B43" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="C43" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D43" s="16">
+        <v>1E-3</v>
+      </c>
+      <c r="E43" s="28"/>
+      <c r="F43" s="28"/>
+      <c r="G43" s="6"/>
+      <c r="H43" s="6"/>
+      <c r="J43" s="12"/>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A44" s="25"/>
+      <c r="B44" s="6"/>
+      <c r="C44" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D44" s="16">
+        <v>0</v>
+      </c>
+      <c r="E44" s="28"/>
+      <c r="F44" s="28"/>
+      <c r="G44" s="6"/>
+      <c r="H44" s="6"/>
+      <c r="J44" s="3"/>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A45" s="25"/>
+      <c r="B45" s="6"/>
+      <c r="C45" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D45" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E45" s="28"/>
+      <c r="F45" s="28"/>
+      <c r="G45" s="6"/>
+      <c r="H45" s="6"/>
+      <c r="I45" s="3"/>
+      <c r="J45" s="3"/>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A46" s="26"/>
+      <c r="B46" s="7"/>
+      <c r="C46" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D46" s="21">
+        <v>0.95</v>
+      </c>
+      <c r="E46" s="29"/>
+      <c r="F46" s="29"/>
+      <c r="G46" s="7"/>
+      <c r="H46" s="7"/>
+      <c r="I46" s="4"/>
+      <c r="J46" s="4"/>
+    </row>
+    <row r="47" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="24" t="s">
+        <v>69</v>
+      </c>
+      <c r="B47" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="C47" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D47" s="20">
+        <v>500</v>
+      </c>
+      <c r="E47" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="F47" s="27" t="s">
+        <v>57</v>
+      </c>
+      <c r="G47" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="H47" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="J47" s="23" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A48" s="25"/>
+      <c r="B48" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="C48" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D48" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="E48" s="28"/>
+      <c r="F48" s="28"/>
+      <c r="G48" s="6"/>
+      <c r="H48" s="6"/>
+      <c r="J48" s="32" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A49" s="25"/>
+      <c r="B49" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="C49" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D49" s="16">
+        <v>1E-3</v>
+      </c>
+      <c r="E49" s="28"/>
+      <c r="F49" s="28"/>
+      <c r="G49" s="6"/>
+      <c r="H49" s="6"/>
+      <c r="J49" s="12" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A50" s="25"/>
+      <c r="B50" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="C50" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D50" s="16">
+        <v>0</v>
+      </c>
+      <c r="E50" s="28"/>
+      <c r="F50" s="28"/>
+      <c r="G50" s="6"/>
+      <c r="H50" s="6"/>
+      <c r="J50" s="3"/>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A51" s="25"/>
+      <c r="B51" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="C51" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D51" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E51" s="28"/>
+      <c r="F51" s="28"/>
+      <c r="G51" s="6"/>
+      <c r="H51" s="6"/>
+      <c r="I51" s="3"/>
+      <c r="J51" s="3"/>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A52" s="26"/>
+      <c r="B52" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="C52" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D52" s="21">
+        <v>0.95</v>
+      </c>
+      <c r="E52" s="29"/>
+      <c r="F52" s="29"/>
+      <c r="G52" s="7"/>
+      <c r="H52" s="7"/>
+      <c r="I52" s="4"/>
+      <c r="J52" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="11">
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="A3:A8"/>
-    <mergeCell ref="A9:A14"/>
-    <mergeCell ref="A15:A20"/>
-    <mergeCell ref="E3:E8"/>
-    <mergeCell ref="I3:I8"/>
-    <mergeCell ref="F3:F8"/>
-    <mergeCell ref="E9:E14"/>
-    <mergeCell ref="F9:F14"/>
-    <mergeCell ref="E15:E20"/>
-    <mergeCell ref="F15:F20"/>
+  <mergeCells count="26">
+    <mergeCell ref="A35:A40"/>
+    <mergeCell ref="E35:E40"/>
+    <mergeCell ref="F35:F40"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="A5:A10"/>
+    <mergeCell ref="A11:A16"/>
+    <mergeCell ref="A17:A22"/>
+    <mergeCell ref="E5:E10"/>
+    <mergeCell ref="A29:A34"/>
+    <mergeCell ref="E29:E34"/>
+    <mergeCell ref="F29:F34"/>
+    <mergeCell ref="A23:A28"/>
+    <mergeCell ref="E23:E28"/>
+    <mergeCell ref="F23:F28"/>
+    <mergeCell ref="I5:I10"/>
+    <mergeCell ref="F5:F10"/>
+    <mergeCell ref="E11:E16"/>
+    <mergeCell ref="F11:F16"/>
+    <mergeCell ref="E17:E22"/>
+    <mergeCell ref="F17:F22"/>
+    <mergeCell ref="A41:A46"/>
+    <mergeCell ref="E41:E46"/>
+    <mergeCell ref="F41:F46"/>
+    <mergeCell ref="A47:A52"/>
+    <mergeCell ref="E47:E52"/>
+    <mergeCell ref="F47:F52"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
- updated the training result.
</commit_message>
<xml_diff>
--- a/training_result.xlsx
+++ b/training_result.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="15405" yWindow="0" windowWidth="19305" windowHeight="8340"/>
+    <workbookView xWindow="20145" yWindow="0" windowWidth="19305" windowHeight="8340"/>
   </bookViews>
   <sheets>
     <sheet name="house_price" sheetId="2" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="90">
   <si>
     <t>Model</t>
   </si>
@@ -412,7 +412,130 @@
     <t>==&gt; more training data (above), more complex model were not helpful</t>
   </si>
   <si>
-    <t>==&gt; The reason may be data processing</t>
+    <t>==&gt; the reason may be data processing</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">data = </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(2,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 301)
+label = (2,)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">data = </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(1458,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 301)
+label = (1458,)</t>
+    </r>
+  </si>
+  <si>
+    <t>Using L2_beta was helpful to reduce eCost</t>
+  </si>
+  <si>
+    <t>result_9</t>
+  </si>
+  <si>
+    <t>min: 0.24146/20~</t>
+  </si>
+  <si>
+    <t>result_10</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">data = </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(1314,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 301)
+label = (1314,)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">data = </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(146,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 301)
+label = (146,)</t>
+    </r>
+  </si>
+  <si>
+    <t>min: 0.29562/9560</t>
   </si>
 </sst>
 </file>
@@ -606,6 +729,16 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -615,22 +748,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -911,10 +1034,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J52"/>
+  <dimension ref="A1:J64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C32" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J40" sqref="J40"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G49" sqref="G49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -947,10 +1070,10 @@
       <c r="B4" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="30" t="s">
+      <c r="C4" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="31"/>
+      <c r="D4" s="32"/>
       <c r="E4" s="9" t="s">
         <v>13</v>
       </c>
@@ -971,7 +1094,7 @@
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="25" t="s">
+      <c r="A5" s="29" t="s">
         <v>19</v>
       </c>
       <c r="B5" s="5" t="s">
@@ -983,23 +1106,23 @@
       <c r="D5" s="5">
         <v>100</v>
       </c>
-      <c r="E5" s="27" t="s">
+      <c r="E5" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="F5" s="27" t="s">
+      <c r="F5" s="25" t="s">
         <v>22</v>
       </c>
       <c r="G5" s="6"/>
       <c r="H5" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="I5" s="27" t="s">
+      <c r="I5" s="25" t="s">
         <v>25</v>
       </c>
       <c r="J5" s="11"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="25"/>
+      <c r="A6" s="29"/>
       <c r="B6" s="6" t="s">
         <v>8</v>
       </c>
@@ -1009,17 +1132,17 @@
       <c r="D6" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="28"/>
-      <c r="F6" s="28"/>
+      <c r="E6" s="26"/>
+      <c r="F6" s="26"/>
       <c r="G6" s="6"/>
       <c r="H6" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="I6" s="28"/>
+      <c r="I6" s="26"/>
       <c r="J6" s="12"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="25"/>
+      <c r="A7" s="29"/>
       <c r="B7" s="6" t="s">
         <v>9</v>
       </c>
@@ -1029,15 +1152,15 @@
       <c r="D7" s="6">
         <v>1E-3</v>
       </c>
-      <c r="E7" s="28"/>
-      <c r="F7" s="28"/>
+      <c r="E7" s="26"/>
+      <c r="F7" s="26"/>
       <c r="G7" s="6"/>
       <c r="H7" s="6"/>
-      <c r="I7" s="28"/>
+      <c r="I7" s="26"/>
       <c r="J7" s="3"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="25"/>
+      <c r="A8" s="29"/>
       <c r="B8" s="6" t="s">
         <v>10</v>
       </c>
@@ -1047,15 +1170,15 @@
       <c r="D8" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E8" s="28"/>
-      <c r="F8" s="28"/>
+      <c r="E8" s="26"/>
+      <c r="F8" s="26"/>
       <c r="G8" s="6"/>
       <c r="H8" s="6"/>
-      <c r="I8" s="28"/>
+      <c r="I8" s="26"/>
       <c r="J8" s="3"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="25"/>
+      <c r="A9" s="29"/>
       <c r="B9" s="6"/>
       <c r="C9" s="6" t="s">
         <v>6</v>
@@ -1063,15 +1186,15 @@
       <c r="D9" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E9" s="28"/>
-      <c r="F9" s="28"/>
+      <c r="E9" s="26"/>
+      <c r="F9" s="26"/>
       <c r="G9" s="6"/>
       <c r="H9" s="6"/>
-      <c r="I9" s="28"/>
+      <c r="I9" s="26"/>
       <c r="J9" s="3"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="25"/>
+      <c r="A10" s="29"/>
       <c r="B10" s="7"/>
       <c r="C10" s="7" t="s">
         <v>20</v>
@@ -1079,15 +1202,15 @@
       <c r="D10" s="7">
         <v>0.99</v>
       </c>
-      <c r="E10" s="29"/>
-      <c r="F10" s="29"/>
+      <c r="E10" s="27"/>
+      <c r="F10" s="27"/>
       <c r="G10" s="7"/>
       <c r="H10" s="7"/>
-      <c r="I10" s="29"/>
+      <c r="I10" s="27"/>
       <c r="J10" s="4"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="24" t="s">
+      <c r="A11" s="28" t="s">
         <v>23</v>
       </c>
       <c r="B11" s="5" t="s">
@@ -1099,10 +1222,10 @@
       <c r="D11" s="5">
         <v>100</v>
       </c>
-      <c r="E11" s="27" t="s">
+      <c r="E11" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="F11" s="27" t="s">
+      <c r="F11" s="25" t="s">
         <v>22</v>
       </c>
       <c r="G11" s="6"/>
@@ -1115,7 +1238,7 @@
       <c r="J11" s="3"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="25"/>
+      <c r="A12" s="29"/>
       <c r="B12" s="6" t="s">
         <v>8</v>
       </c>
@@ -1125,8 +1248,8 @@
       <c r="D12" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="E12" s="28"/>
-      <c r="F12" s="28"/>
+      <c r="E12" s="26"/>
+      <c r="F12" s="26"/>
       <c r="G12" s="6"/>
       <c r="H12" s="6"/>
       <c r="I12" t="s">
@@ -1135,7 +1258,7 @@
       <c r="J12" s="3"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="25"/>
+      <c r="A13" s="29"/>
       <c r="B13" s="6" t="s">
         <v>9</v>
       </c>
@@ -1145,8 +1268,8 @@
       <c r="D13" s="6">
         <v>1E-3</v>
       </c>
-      <c r="E13" s="28"/>
-      <c r="F13" s="28"/>
+      <c r="E13" s="26"/>
+      <c r="F13" s="26"/>
       <c r="G13" s="6"/>
       <c r="H13" s="6"/>
       <c r="I13" t="s">
@@ -1155,7 +1278,7 @@
       <c r="J13" s="3"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="25"/>
+      <c r="A14" s="29"/>
       <c r="B14" s="6" t="s">
         <v>10</v>
       </c>
@@ -1165,8 +1288,8 @@
       <c r="D14" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E14" s="28"/>
-      <c r="F14" s="28"/>
+      <c r="E14" s="26"/>
+      <c r="F14" s="26"/>
       <c r="G14" s="6"/>
       <c r="H14" s="6"/>
       <c r="I14" t="s">
@@ -1175,7 +1298,7 @@
       <c r="J14" s="3"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="25"/>
+      <c r="A15" s="29"/>
       <c r="B15" s="6"/>
       <c r="C15" s="6" t="s">
         <v>6</v>
@@ -1183,8 +1306,8 @@
       <c r="D15" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E15" s="28"/>
-      <c r="F15" s="28"/>
+      <c r="E15" s="26"/>
+      <c r="F15" s="26"/>
       <c r="G15" s="6"/>
       <c r="H15" s="6"/>
       <c r="I15" t="s">
@@ -1193,7 +1316,7 @@
       <c r="J15" s="3"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="26"/>
+      <c r="A16" s="30"/>
       <c r="B16" s="7"/>
       <c r="C16" s="7" t="s">
         <v>20</v>
@@ -1201,15 +1324,15 @@
       <c r="D16" s="7">
         <v>0.99</v>
       </c>
-      <c r="E16" s="29"/>
-      <c r="F16" s="29"/>
+      <c r="E16" s="27"/>
+      <c r="F16" s="27"/>
       <c r="G16" s="7"/>
       <c r="H16" s="7"/>
       <c r="I16" s="4"/>
       <c r="J16" s="4"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="25" t="s">
+      <c r="A17" s="29" t="s">
         <v>24</v>
       </c>
       <c r="B17" s="5" t="s">
@@ -1221,10 +1344,10 @@
       <c r="D17" s="5">
         <v>500</v>
       </c>
-      <c r="E17" s="27" t="s">
+      <c r="E17" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="F17" s="27" t="s">
+      <c r="F17" s="25" t="s">
         <v>22</v>
       </c>
       <c r="G17" s="6"/>
@@ -1235,7 +1358,7 @@
       <c r="J17" s="2"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="25"/>
+      <c r="A18" s="29"/>
       <c r="B18" s="6" t="s">
         <v>8</v>
       </c>
@@ -1245,15 +1368,15 @@
       <c r="D18" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="E18" s="28"/>
-      <c r="F18" s="28"/>
+      <c r="E18" s="26"/>
+      <c r="F18" s="26"/>
       <c r="G18" s="6"/>
       <c r="H18" s="6"/>
       <c r="I18" s="3"/>
       <c r="J18" s="3"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="25"/>
+      <c r="A19" s="29"/>
       <c r="B19" s="6" t="s">
         <v>9</v>
       </c>
@@ -1263,15 +1386,15 @@
       <c r="D19" s="6">
         <v>1E-3</v>
       </c>
-      <c r="E19" s="28"/>
-      <c r="F19" s="28"/>
+      <c r="E19" s="26"/>
+      <c r="F19" s="26"/>
       <c r="G19" s="6"/>
       <c r="H19" s="6"/>
       <c r="I19" s="3"/>
       <c r="J19" s="3"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="25"/>
+      <c r="A20" s="29"/>
       <c r="B20" s="6" t="s">
         <v>10</v>
       </c>
@@ -1281,15 +1404,15 @@
       <c r="D20" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E20" s="28"/>
-      <c r="F20" s="28"/>
+      <c r="E20" s="26"/>
+      <c r="F20" s="26"/>
       <c r="G20" s="6"/>
       <c r="H20" s="6"/>
       <c r="I20" s="3"/>
       <c r="J20" s="3"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="25"/>
+      <c r="A21" s="29"/>
       <c r="B21" s="6"/>
       <c r="C21" s="6" t="s">
         <v>6</v>
@@ -1297,15 +1420,15 @@
       <c r="D21" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E21" s="28"/>
-      <c r="F21" s="28"/>
+      <c r="E21" s="26"/>
+      <c r="F21" s="26"/>
       <c r="G21" s="6"/>
       <c r="H21" s="6"/>
       <c r="I21" s="3"/>
       <c r="J21" s="3"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="25"/>
+      <c r="A22" s="29"/>
       <c r="B22" s="7"/>
       <c r="C22" s="7" t="s">
         <v>20</v>
@@ -1313,15 +1436,15 @@
       <c r="D22" s="7">
         <v>0.99</v>
       </c>
-      <c r="E22" s="29"/>
-      <c r="F22" s="29"/>
+      <c r="E22" s="27"/>
+      <c r="F22" s="27"/>
       <c r="G22" s="7"/>
       <c r="H22" s="7"/>
       <c r="I22" s="4"/>
       <c r="J22" s="4"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="24" t="s">
+      <c r="A23" s="28" t="s">
         <v>39</v>
       </c>
       <c r="B23" s="5" t="s">
@@ -1333,10 +1456,10 @@
       <c r="D23" s="18">
         <v>500</v>
       </c>
-      <c r="E23" s="27" t="s">
+      <c r="E23" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="F23" s="27" t="s">
+      <c r="F23" s="25" t="s">
         <v>41</v>
       </c>
       <c r="G23" s="6" t="s">
@@ -1353,7 +1476,7 @@
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" s="25"/>
+      <c r="A24" s="29"/>
       <c r="B24" s="6" t="s">
         <v>8</v>
       </c>
@@ -1363,8 +1486,8 @@
       <c r="D24" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="E24" s="28"/>
-      <c r="F24" s="28"/>
+      <c r="E24" s="26"/>
+      <c r="F24" s="26"/>
       <c r="G24" s="6"/>
       <c r="H24" s="6"/>
       <c r="I24" t="s">
@@ -1375,7 +1498,7 @@
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" s="25"/>
+      <c r="A25" s="29"/>
       <c r="B25" s="6" t="s">
         <v>9</v>
       </c>
@@ -1385,8 +1508,8 @@
       <c r="D25" s="6">
         <v>1E-3</v>
       </c>
-      <c r="E25" s="28"/>
-      <c r="F25" s="28"/>
+      <c r="E25" s="26"/>
+      <c r="F25" s="26"/>
       <c r="G25" s="6"/>
       <c r="H25" s="6"/>
       <c r="I25" t="s">
@@ -1395,7 +1518,7 @@
       <c r="J25" s="3"/>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" s="25"/>
+      <c r="A26" s="29"/>
       <c r="B26" s="6" t="s">
         <v>10</v>
       </c>
@@ -1405,8 +1528,8 @@
       <c r="D26" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E26" s="28"/>
-      <c r="F26" s="28"/>
+      <c r="E26" s="26"/>
+      <c r="F26" s="26"/>
       <c r="G26" s="6"/>
       <c r="H26" s="6"/>
       <c r="I26" t="s">
@@ -1415,7 +1538,7 @@
       <c r="J26" s="3"/>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" s="25"/>
+      <c r="A27" s="29"/>
       <c r="B27" s="6"/>
       <c r="C27" s="6" t="s">
         <v>6</v>
@@ -1423,15 +1546,15 @@
       <c r="D27" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E27" s="28"/>
-      <c r="F27" s="28"/>
+      <c r="E27" s="26"/>
+      <c r="F27" s="26"/>
       <c r="G27" s="6"/>
       <c r="H27" s="6"/>
       <c r="I27" s="3"/>
       <c r="J27" s="3"/>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28" s="26"/>
+      <c r="A28" s="30"/>
       <c r="B28" s="7"/>
       <c r="C28" s="7" t="s">
         <v>20</v>
@@ -1439,15 +1562,15 @@
       <c r="D28" s="19">
         <v>0.8</v>
       </c>
-      <c r="E28" s="29"/>
-      <c r="F28" s="29"/>
+      <c r="E28" s="27"/>
+      <c r="F28" s="27"/>
       <c r="G28" s="7"/>
       <c r="H28" s="7"/>
       <c r="I28" s="4"/>
       <c r="J28" s="4"/>
     </row>
     <row r="29" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="24" t="s">
+      <c r="A29" s="28" t="s">
         <v>50</v>
       </c>
       <c r="B29" s="5" t="s">
@@ -1459,10 +1582,10 @@
       <c r="D29" s="20">
         <v>500</v>
       </c>
-      <c r="E29" s="27" t="s">
+      <c r="E29" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="F29" s="27" t="s">
+      <c r="F29" s="25" t="s">
         <v>41</v>
       </c>
       <c r="G29" s="13" t="s">
@@ -1476,7 +1599,7 @@
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A30" s="25"/>
+      <c r="A30" s="29"/>
       <c r="B30" s="6" t="s">
         <v>8</v>
       </c>
@@ -1486,8 +1609,8 @@
       <c r="D30" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="E30" s="28"/>
-      <c r="F30" s="28"/>
+      <c r="E30" s="26"/>
+      <c r="F30" s="26"/>
       <c r="G30" s="6"/>
       <c r="H30" s="6"/>
       <c r="J30" s="12" t="s">
@@ -1495,7 +1618,7 @@
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31" s="25"/>
+      <c r="A31" s="29"/>
       <c r="B31" s="6" t="s">
         <v>9</v>
       </c>
@@ -1505,14 +1628,14 @@
       <c r="D31" s="17">
         <v>1E-4</v>
       </c>
-      <c r="E31" s="28"/>
-      <c r="F31" s="28"/>
+      <c r="E31" s="26"/>
+      <c r="F31" s="26"/>
       <c r="G31" s="6"/>
       <c r="H31" s="6"/>
       <c r="J31" s="3"/>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A32" s="25"/>
+      <c r="A32" s="29"/>
       <c r="B32" s="6" t="s">
         <v>10</v>
       </c>
@@ -1522,14 +1645,14 @@
       <c r="D32" s="17">
         <v>0.9</v>
       </c>
-      <c r="E32" s="28"/>
-      <c r="F32" s="28"/>
+      <c r="E32" s="26"/>
+      <c r="F32" s="26"/>
       <c r="G32" s="6"/>
       <c r="H32" s="6"/>
       <c r="J32" s="3"/>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A33" s="25"/>
+      <c r="A33" s="29"/>
       <c r="B33" s="6"/>
       <c r="C33" s="6" t="s">
         <v>6</v>
@@ -1537,15 +1660,15 @@
       <c r="D33" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E33" s="28"/>
-      <c r="F33" s="28"/>
+      <c r="E33" s="26"/>
+      <c r="F33" s="26"/>
       <c r="G33" s="6"/>
       <c r="H33" s="6"/>
       <c r="I33" s="3"/>
       <c r="J33" s="3"/>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A34" s="26"/>
+      <c r="A34" s="30"/>
       <c r="B34" s="7"/>
       <c r="C34" s="7" t="s">
         <v>20</v>
@@ -1553,15 +1676,15 @@
       <c r="D34" s="21">
         <v>0.8</v>
       </c>
-      <c r="E34" s="29"/>
-      <c r="F34" s="29"/>
+      <c r="E34" s="27"/>
+      <c r="F34" s="27"/>
       <c r="G34" s="7"/>
       <c r="H34" s="7"/>
       <c r="I34" s="4"/>
       <c r="J34" s="4"/>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A35" s="24" t="s">
+      <c r="A35" s="28" t="s">
         <v>54</v>
       </c>
       <c r="B35" s="5" t="s">
@@ -1573,10 +1696,10 @@
       <c r="D35" s="20">
         <v>500</v>
       </c>
-      <c r="E35" s="27" t="s">
+      <c r="E35" s="25" t="s">
         <v>56</v>
       </c>
-      <c r="F35" s="27" t="s">
+      <c r="F35" s="25" t="s">
         <v>57</v>
       </c>
       <c r="G35" s="13" t="s">
@@ -1590,7 +1713,7 @@
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A36" s="25"/>
+      <c r="A36" s="29"/>
       <c r="B36" s="6" t="s">
         <v>8</v>
       </c>
@@ -1600,8 +1723,8 @@
       <c r="D36" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="E36" s="28"/>
-      <c r="F36" s="28"/>
+      <c r="E36" s="26"/>
+      <c r="F36" s="26"/>
       <c r="G36" s="6"/>
       <c r="H36" s="6"/>
       <c r="J36" s="22" t="s">
@@ -1609,7 +1732,7 @@
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A37" s="25"/>
+      <c r="A37" s="29"/>
       <c r="B37" s="6" t="s">
         <v>9</v>
       </c>
@@ -1619,8 +1742,8 @@
       <c r="D37" s="16">
         <v>1E-3</v>
       </c>
-      <c r="E37" s="28"/>
-      <c r="F37" s="28"/>
+      <c r="E37" s="26"/>
+      <c r="F37" s="26"/>
       <c r="G37" s="6"/>
       <c r="H37" s="6"/>
       <c r="J37" s="12" t="s">
@@ -1628,7 +1751,7 @@
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A38" s="25"/>
+      <c r="A38" s="29"/>
       <c r="B38" s="6" t="s">
         <v>10</v>
       </c>
@@ -1638,14 +1761,14 @@
       <c r="D38" s="16">
         <v>0</v>
       </c>
-      <c r="E38" s="28"/>
-      <c r="F38" s="28"/>
+      <c r="E38" s="26"/>
+      <c r="F38" s="26"/>
       <c r="G38" s="6"/>
       <c r="H38" s="6"/>
       <c r="J38" s="3"/>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A39" s="25"/>
+      <c r="A39" s="29"/>
       <c r="B39" s="6"/>
       <c r="C39" s="6" t="s">
         <v>6</v>
@@ -1653,15 +1776,15 @@
       <c r="D39" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E39" s="28"/>
-      <c r="F39" s="28"/>
+      <c r="E39" s="26"/>
+      <c r="F39" s="26"/>
       <c r="G39" s="6"/>
       <c r="H39" s="6"/>
       <c r="I39" s="3"/>
       <c r="J39" s="3"/>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A40" s="26"/>
+      <c r="A40" s="30"/>
       <c r="B40" s="7"/>
       <c r="C40" s="7" t="s">
         <v>20</v>
@@ -1669,15 +1792,15 @@
       <c r="D40" s="19">
         <v>0.95</v>
       </c>
-      <c r="E40" s="29"/>
-      <c r="F40" s="29"/>
+      <c r="E40" s="27"/>
+      <c r="F40" s="27"/>
       <c r="G40" s="7"/>
       <c r="H40" s="7"/>
       <c r="I40" s="4"/>
       <c r="J40" s="4"/>
     </row>
     <row r="41" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="24" t="s">
+      <c r="A41" s="28" t="s">
         <v>63</v>
       </c>
       <c r="B41" s="6" t="s">
@@ -1689,10 +1812,10 @@
       <c r="D41" s="20">
         <v>500</v>
       </c>
-      <c r="E41" s="27" t="s">
+      <c r="E41" s="25" t="s">
         <v>56</v>
       </c>
-      <c r="F41" s="27" t="s">
+      <c r="F41" s="25" t="s">
         <v>57</v>
       </c>
       <c r="G41" s="13" t="s">
@@ -1704,7 +1827,7 @@
       <c r="J41" s="23"/>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A42" s="25"/>
+      <c r="A42" s="29"/>
       <c r="B42" s="6" t="s">
         <v>65</v>
       </c>
@@ -1714,14 +1837,14 @@
       <c r="D42" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="E42" s="28"/>
-      <c r="F42" s="28"/>
+      <c r="E42" s="26"/>
+      <c r="F42" s="26"/>
       <c r="G42" s="6"/>
       <c r="H42" s="6"/>
       <c r="J42" s="22"/>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A43" s="25"/>
+      <c r="A43" s="29"/>
       <c r="B43" s="6" t="s">
         <v>66</v>
       </c>
@@ -1731,14 +1854,14 @@
       <c r="D43" s="16">
         <v>1E-3</v>
       </c>
-      <c r="E43" s="28"/>
-      <c r="F43" s="28"/>
+      <c r="E43" s="26"/>
+      <c r="F43" s="26"/>
       <c r="G43" s="6"/>
       <c r="H43" s="6"/>
       <c r="J43" s="12"/>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A44" s="25"/>
+      <c r="A44" s="29"/>
       <c r="B44" s="6"/>
       <c r="C44" s="6" t="s">
         <v>5</v>
@@ -1746,14 +1869,14 @@
       <c r="D44" s="16">
         <v>0</v>
       </c>
-      <c r="E44" s="28"/>
-      <c r="F44" s="28"/>
+      <c r="E44" s="26"/>
+      <c r="F44" s="26"/>
       <c r="G44" s="6"/>
       <c r="H44" s="6"/>
       <c r="J44" s="3"/>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A45" s="25"/>
+      <c r="A45" s="29"/>
       <c r="B45" s="6"/>
       <c r="C45" s="6" t="s">
         <v>6</v>
@@ -1761,15 +1884,15 @@
       <c r="D45" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E45" s="28"/>
-      <c r="F45" s="28"/>
+      <c r="E45" s="26"/>
+      <c r="F45" s="26"/>
       <c r="G45" s="6"/>
       <c r="H45" s="6"/>
       <c r="I45" s="3"/>
       <c r="J45" s="3"/>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A46" s="26"/>
+      <c r="A46" s="30"/>
       <c r="B46" s="7"/>
       <c r="C46" s="7" t="s">
         <v>20</v>
@@ -1777,15 +1900,15 @@
       <c r="D46" s="21">
         <v>0.95</v>
       </c>
-      <c r="E46" s="29"/>
-      <c r="F46" s="29"/>
+      <c r="E46" s="27"/>
+      <c r="F46" s="27"/>
       <c r="G46" s="7"/>
       <c r="H46" s="7"/>
       <c r="I46" s="4"/>
       <c r="J46" s="4"/>
     </row>
     <row r="47" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="24" t="s">
+      <c r="A47" s="28" t="s">
         <v>69</v>
       </c>
       <c r="B47" s="6" t="s">
@@ -1797,10 +1920,10 @@
       <c r="D47" s="20">
         <v>500</v>
       </c>
-      <c r="E47" s="27" t="s">
+      <c r="E47" s="25" t="s">
         <v>56</v>
       </c>
-      <c r="F47" s="27" t="s">
+      <c r="F47" s="25" t="s">
         <v>57</v>
       </c>
       <c r="G47" s="13" t="s">
@@ -1814,7 +1937,7 @@
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A48" s="25"/>
+      <c r="A48" s="29"/>
       <c r="B48" s="6" t="s">
         <v>71</v>
       </c>
@@ -1824,16 +1947,16 @@
       <c r="D48" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="E48" s="28"/>
-      <c r="F48" s="28"/>
+      <c r="E48" s="26"/>
+      <c r="F48" s="26"/>
       <c r="G48" s="6"/>
       <c r="H48" s="6"/>
-      <c r="J48" s="32" t="s">
+      <c r="J48" s="24" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A49" s="25"/>
+      <c r="A49" s="29"/>
       <c r="B49" s="6" t="s">
         <v>72</v>
       </c>
@@ -1843,8 +1966,8 @@
       <c r="D49" s="16">
         <v>1E-3</v>
       </c>
-      <c r="E49" s="28"/>
-      <c r="F49" s="28"/>
+      <c r="E49" s="26"/>
+      <c r="F49" s="26"/>
       <c r="G49" s="6"/>
       <c r="H49" s="6"/>
       <c r="J49" s="12" t="s">
@@ -1852,7 +1975,7 @@
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A50" s="25"/>
+      <c r="A50" s="29"/>
       <c r="B50" s="6" t="s">
         <v>73</v>
       </c>
@@ -1862,14 +1985,14 @@
       <c r="D50" s="16">
         <v>0</v>
       </c>
-      <c r="E50" s="28"/>
-      <c r="F50" s="28"/>
+      <c r="E50" s="26"/>
+      <c r="F50" s="26"/>
       <c r="G50" s="6"/>
       <c r="H50" s="6"/>
       <c r="J50" s="3"/>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A51" s="25"/>
+      <c r="A51" s="29"/>
       <c r="B51" s="6" t="s">
         <v>74</v>
       </c>
@@ -1879,15 +2002,15 @@
       <c r="D51" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E51" s="28"/>
-      <c r="F51" s="28"/>
+      <c r="E51" s="26"/>
+      <c r="F51" s="26"/>
       <c r="G51" s="6"/>
       <c r="H51" s="6"/>
       <c r="I51" s="3"/>
       <c r="J51" s="3"/>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A52" s="26"/>
+      <c r="A52" s="30"/>
       <c r="B52" s="7" t="s">
         <v>75</v>
       </c>
@@ -1897,18 +2020,256 @@
       <c r="D52" s="21">
         <v>0.95</v>
       </c>
-      <c r="E52" s="29"/>
-      <c r="F52" s="29"/>
+      <c r="E52" s="27"/>
+      <c r="F52" s="27"/>
       <c r="G52" s="7"/>
       <c r="H52" s="7"/>
       <c r="I52" s="4"/>
       <c r="J52" s="4"/>
     </row>
+    <row r="53" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="28" t="s">
+        <v>84</v>
+      </c>
+      <c r="B53" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="C53" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D53" s="20">
+        <v>500</v>
+      </c>
+      <c r="E53" s="25" t="s">
+        <v>82</v>
+      </c>
+      <c r="F53" s="25" t="s">
+        <v>81</v>
+      </c>
+      <c r="G53" s="13"/>
+      <c r="H53" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="J53" s="23" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A54" s="29"/>
+      <c r="B54" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="C54" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D54" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="E54" s="26"/>
+      <c r="F54" s="26"/>
+      <c r="G54" s="6"/>
+      <c r="H54" s="6"/>
+      <c r="J54" s="24"/>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A55" s="29"/>
+      <c r="B55" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="C55" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D55" s="16">
+        <v>1E-3</v>
+      </c>
+      <c r="E55" s="26"/>
+      <c r="F55" s="26"/>
+      <c r="G55" s="6"/>
+      <c r="H55" s="6"/>
+      <c r="J55" s="12"/>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A56" s="29"/>
+      <c r="B56" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="C56" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D56" s="16">
+        <v>0</v>
+      </c>
+      <c r="E56" s="26"/>
+      <c r="F56" s="26"/>
+      <c r="G56" s="6"/>
+      <c r="H56" s="6"/>
+      <c r="J56" s="3"/>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A57" s="29"/>
+      <c r="B57" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="C57" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D57" s="17">
+        <v>1E-3</v>
+      </c>
+      <c r="E57" s="26"/>
+      <c r="F57" s="26"/>
+      <c r="G57" s="6"/>
+      <c r="H57" s="6"/>
+      <c r="I57" s="3"/>
+      <c r="J57" s="3"/>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A58" s="30"/>
+      <c r="B58" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="C58" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D58" s="21">
+        <v>0.99</v>
+      </c>
+      <c r="E58" s="27"/>
+      <c r="F58" s="27"/>
+      <c r="G58" s="7"/>
+      <c r="H58" s="7"/>
+      <c r="I58" s="4"/>
+      <c r="J58" s="4"/>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A59" s="28" t="s">
+        <v>86</v>
+      </c>
+      <c r="B59" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="C59" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D59" s="20">
+        <v>500</v>
+      </c>
+      <c r="E59" s="25" t="s">
+        <v>87</v>
+      </c>
+      <c r="F59" s="25" t="s">
+        <v>88</v>
+      </c>
+      <c r="G59" s="13"/>
+      <c r="H59" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="J59" s="23"/>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A60" s="29"/>
+      <c r="B60" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="C60" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D60" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="E60" s="26"/>
+      <c r="F60" s="26"/>
+      <c r="G60" s="6"/>
+      <c r="H60" s="6"/>
+      <c r="J60" s="24"/>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A61" s="29"/>
+      <c r="B61" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="C61" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D61" s="16">
+        <v>1E-3</v>
+      </c>
+      <c r="E61" s="26"/>
+      <c r="F61" s="26"/>
+      <c r="G61" s="6"/>
+      <c r="H61" s="6"/>
+      <c r="J61" s="12"/>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A62" s="29"/>
+      <c r="B62" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="C62" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D62" s="16">
+        <v>0</v>
+      </c>
+      <c r="E62" s="26"/>
+      <c r="F62" s="26"/>
+      <c r="G62" s="6"/>
+      <c r="H62" s="6"/>
+      <c r="J62" s="3"/>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A63" s="29"/>
+      <c r="B63" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="C63" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D63" s="17">
+        <v>1E-3</v>
+      </c>
+      <c r="E63" s="26"/>
+      <c r="F63" s="26"/>
+      <c r="G63" s="6"/>
+      <c r="H63" s="6"/>
+      <c r="I63" s="3"/>
+      <c r="J63" s="3"/>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A64" s="30"/>
+      <c r="B64" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="C64" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D64" s="21">
+        <v>0.9</v>
+      </c>
+      <c r="E64" s="27"/>
+      <c r="F64" s="27"/>
+      <c r="G64" s="7"/>
+      <c r="H64" s="7"/>
+      <c r="I64" s="4"/>
+      <c r="J64" s="4"/>
+    </row>
   </sheetData>
-  <mergeCells count="26">
+  <mergeCells count="32">
+    <mergeCell ref="A59:A64"/>
+    <mergeCell ref="E59:E64"/>
+    <mergeCell ref="F59:F64"/>
+    <mergeCell ref="E53:E58"/>
+    <mergeCell ref="F53:F58"/>
+    <mergeCell ref="A53:A58"/>
     <mergeCell ref="A35:A40"/>
     <mergeCell ref="E35:E40"/>
     <mergeCell ref="F35:F40"/>
+    <mergeCell ref="A41:A46"/>
+    <mergeCell ref="E41:E46"/>
+    <mergeCell ref="F41:F46"/>
+    <mergeCell ref="A47:A52"/>
+    <mergeCell ref="E47:E52"/>
+    <mergeCell ref="F47:F52"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="A5:A10"/>
     <mergeCell ref="A11:A16"/>
@@ -1926,12 +2287,6 @@
     <mergeCell ref="F11:F16"/>
     <mergeCell ref="E17:E22"/>
     <mergeCell ref="F17:F22"/>
-    <mergeCell ref="A41:A46"/>
-    <mergeCell ref="E41:E46"/>
-    <mergeCell ref="F41:F46"/>
-    <mergeCell ref="A47:A52"/>
-    <mergeCell ref="E47:E52"/>
-    <mergeCell ref="F47:F52"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>